<commit_message>
Moloy Traits (Continued) 업데이트
#679
</commit_message>
<xml_diff>
--- a/Data/Mlie/Moloy Traits (Continued) - 2566452140/2566452140.xlsx
+++ b/Data/Mlie/Moloy Traits (Continued) - 2566452140/2566452140.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.11\Moloy Traits (Continued) - 2566452140\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Mlie\Moloy Traits (Continued) - 2566452140\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4299A49-A2A4-41F6-8311-FFE591928067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9689EE5D-9732-42A4-9128-E3A86B805DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240415" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240416" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="262">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -524,200 +524,306 @@
     <t>TraitDef+MT_Commander.degreeDatas.0.label</t>
   </si>
   <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Commander.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Commander.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} is an effective leader in ranged combat. Colonists around {PAWN_nameDef} have better aim.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Hermit.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Hermit.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Hermit</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Hermit.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Hermit.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} prefers being solitary. {PAWN_pronoun} is better at working with plants anyways.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Peppy.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Peppy.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Peppy</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Peppy.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Peppy.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} is full of energy. {PAWN_pronoun} will randomly gain the Frenzy Go Inspiration, even if {PAWN_pronoun} is not happy.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Volatile_Crafter.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Volatile_Crafter.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Volatile Crafter</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Volatile_Crafter.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Volatile_Crafter.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} is a genius crafter, and will often have creative inspiration. However, {PAWN_possessive} mind is constantly ticking, making {PAWN_nameDef} much more likely to have a mental break.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Luminary.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Luminary.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Luminary</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Luminary.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Luminary.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>For whatever reason, everyone seems to really care how {PAWN_nameDef} is feeling.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Tyrant.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Tyrant.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Tyrannic</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Tyrant.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Tyrant.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} harshly criticizes and dictates the actions of others. Colonists around {PAWN_nameDef} move and work faster, but receive a mood debuff from the added stress.</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Venturous.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>MT_Venturous.degreeDatas.0.label</t>
+  </si>
+  <si>
+    <t>Venturous</t>
+  </si>
+  <si>
+    <t>TraitDef+MT_Venturous.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>MT_Venturous.degreeDatas.0.description</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef} loves to take risks and complete quests. {PAWN_pronoun} will recieve mood buffs for successful quests, and debuffs for failed quests.</t>
+  </si>
+  <si>
+    <t>모험적</t>
+  </si>
+  <si>
+    <t>폭군</t>
+  </si>
+  <si>
+    <t>사소한 일 하나하나가 지적당하고 비난당하고 있어, 그냥 나를 내버려 둬!</t>
+  </si>
+  <si>
+    <t>폭군의 근처</t>
+  </si>
+  <si>
+    <t>임무를 끝낸 지 좀 됐어. 어서 해치우자고.</t>
+  </si>
+  <si>
+    <t>임무 결과 없음</t>
+  </si>
+  <si>
+    <t>임무를 끝낸 지 오래 됐어. 위험을 감수하지 않는 건 지루해!</t>
+  </si>
+  <si>
+    <t>임무를 끝낸 지 너무 오래 됐어. 우린 당장 뭐라도 해야 해!</t>
+  </si>
+  <si>
+    <t>마지막으로 끝낸 임무가 기억이 안 나. 인생이 따분하고 의미가 없어.</t>
+  </si>
+  <si>
+    <t>최근에 우리는 엄청난 양의 임무를 성공했어, 여긴 정말 끝내줘!</t>
+  </si>
+  <si>
+    <t>임무 성공</t>
+  </si>
+  <si>
+    <t>최근에 우리는 몇몇 임무를 성공했어, 정말 놀라워!</t>
+  </si>
+  <si>
+    <t>최근에 우리는 임무를 성공했어, 잘 되어가고 있어.</t>
+  </si>
+  <si>
+    <t>최근에 우리는 임무를 실패했어, 짜증나.</t>
+  </si>
+  <si>
+    <t>임무 실패</t>
+  </si>
+  <si>
+    <t>최근에 우리는 몇몇 임무를 실패했어, 이건 좋지 않아.</t>
+  </si>
+  <si>
+    <t>최근에 우리는 너무 많은 임무를 실패했어, 이건 끔찍해!</t>
+  </si>
+  <si>
+    <t>최근에 우리는 엄청난 양의 임무를 실패했어, 정말 장난같지도 않아.</t>
+  </si>
+  <si>
+    <t>근처의 폭군</t>
+  </si>
+  <si>
+    <t>다른 사람들이 더 빠르게 움직이고 일하라는 가혹한 지시를 받습니다. 스트레스가 늘고, 기분에 부정적인 영향을 끼칩니다.</t>
+  </si>
+  <si>
+    <t>폭군이 가까이에 있음</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>MT_Commander.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Commander</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Commander.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Commander.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} is an effective leader in ranged combat. Colonists around {PAWN_nameDef} have better aim.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Hermit.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Hermit.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Hermit</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Hermit.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Hermit.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} prefers being solitary. {PAWN_pronoun} is better at working with plants anyways.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Peppy.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Peppy.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Peppy</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Peppy.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Peppy.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} is full of energy. {PAWN_pronoun} will randomly gain the Frenzy Go Inspiration, even if {PAWN_pronoun} is not happy.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Volatile_Crafter.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Volatile_Crafter.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Volatile Crafter</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Volatile_Crafter.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Volatile_Crafter.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} is a genius crafter, and will often have creative inspiration. However, {PAWN_possessive} mind is constantly ticking, making {PAWN_nameDef} much more likely to have a mental break.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Luminary.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Luminary.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Luminary</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Luminary.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Luminary.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>For whatever reason, everyone seems to really care how {PAWN_nameDef} is feeling.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Tyrant.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Tyrant.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Tyrannic</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Tyrant.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Tyrant.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} harshly criticizes and dictates the actions of others. Colonists around {PAWN_nameDef} move and work faster, but receive a mood debuff from the added stress.</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Venturous.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>MT_Venturous.degreeDatas.0.label</t>
-  </si>
-  <si>
-    <t>Venturous</t>
-  </si>
-  <si>
-    <t>TraitDef+MT_Venturous.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>MT_Venturous.degreeDatas.0.description</t>
-  </si>
-  <si>
-    <t>{PAWN_nameDef} loves to take risks and complete quests. {PAWN_pronoun} will recieve mood buffs for successful quests, and debuffs for failed quests.</t>
-  </si>
-  <si>
-    <t>모험적</t>
-  </si>
-  <si>
-    <t>폭군</t>
-  </si>
-  <si>
-    <t>사소한 일 하나하나가 지적당하고 비난당하고 있어, 그냥 나를 내버려 둬!</t>
-  </si>
-  <si>
-    <t>폭군의 근처</t>
-  </si>
-  <si>
-    <t>임무를 끝낸 지 좀 됐어. 어서 해치우자고.</t>
-  </si>
-  <si>
-    <t>임무 결과 없음</t>
-  </si>
-  <si>
-    <t>임무를 끝낸 지 오래 됐어. 위험을 감수하지 않는 건 지루해!</t>
-  </si>
-  <si>
-    <t>임무를 끝낸 지 너무 오래 됐어. 우린 당장 뭐라도 해야 해!</t>
-  </si>
-  <si>
-    <t>마지막으로 끝낸 임무가 기억이 안 나. 인생이 따분하고 의미가 없어.</t>
-  </si>
-  <si>
-    <t>최근에 우리는 엄청난 양의 임무를 성공했어, 여긴 정말 끝내줘!</t>
-  </si>
-  <si>
-    <t>임무 성공</t>
-  </si>
-  <si>
-    <t>최근에 우리는 몇몇 임무를 성공했어, 정말 놀라워!</t>
-  </si>
-  <si>
-    <t>최근에 우리는 임무를 성공했어, 잘 되어가고 있어.</t>
-  </si>
-  <si>
-    <t>최근에 우리는 임무를 실패했어, 짜증나.</t>
-  </si>
-  <si>
-    <t>임무 실패</t>
-  </si>
-  <si>
-    <t>최근에 우리는 몇몇 임무를 실패했어, 이건 좋지 않아.</t>
-  </si>
-  <si>
-    <t>최근에 우리는 너무 많은 임무를 실패했어, 이건 끔찍해!</t>
-  </si>
-  <si>
-    <t>최근에 우리는 엄청난 양의 임무를 실패했어, 정말 장난같지도 않아.</t>
-  </si>
-  <si>
-    <t>근처의 폭군</t>
-  </si>
-  <si>
-    <t>다른 사람들이 더 빠르게 움직이고 일하라는 가혹한 지시를 받습니다. 스트레스가 늘고, 기분에 부정적인 영향을 끼칩니다.</t>
-  </si>
-  <si>
-    <t>폭군이 가까이에 있음</t>
-  </si>
-  <si>
-    <t/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지휘관이 가까이에 있음</t>
+  </si>
+  <si>
+    <t>가까운 지휘관</t>
+  </si>
+  <si>
+    <t>지도자가 가까이에 있음</t>
+  </si>
+  <si>
+    <t>가까운 지도자</t>
+  </si>
+  <si>
+    <t>선각자가 너무 불행해하고있어. 이건 날 너무 화나게 만들어!</t>
+  </si>
+  <si>
+    <t>매우 불행한 선각자</t>
+  </si>
+  <si>
+    <t>선각자가 불행해하고있어. 이건 날 화나게 만들어!</t>
+  </si>
+  <si>
+    <t>불행한 선각자</t>
+  </si>
+  <si>
+    <t>선각자가 기분이 좋은가봐. 나도 기분이 좋아지는데!</t>
+  </si>
+  <si>
+    <t>행복한 선각자</t>
+  </si>
+  <si>
+    <t>선각자가 매우 행복해하고있어. 나도 기분이 아주 좋아!</t>
+  </si>
+  <si>
+    <t>매우 행복한 선각자</t>
+  </si>
+  <si>
+    <t>내 전 애인이 떠나버렸어... 난 여전히 외로워! 너무 불공평해. 참을 수가 없어!</t>
+  </si>
+  <si>
+    <t>내 전 애인이 떠남!</t>
+  </si>
+  <si>
+    <t>난 새로운 사랑을 찾았고, 내 전 애인은 여전히 혼자야! 난 너무나 행복해!</t>
+  </si>
+  <si>
+    <t>새로운 사랑을 찾음</t>
+  </si>
+  <si>
+    <t>매력적인</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 전투에서 효과적인 지휘관입니다. {PAWN_possessive} 주변에 있는 정착민들은 목표를 조준하기 더 쉬워집니다.</t>
+  </si>
+  <si>
+    <t>지휘관</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 다른 사람들의 행동을 잘 이끌어내는 편입니다. {PAWN_possessive} 주변에 있는 정착민들은 더욱 빨리 움직입니다.</t>
+  </si>
+  <si>
+    <t>지도자</t>
+  </si>
+  <si>
+    <t>괴짜</t>
+  </si>
+  <si>
+    <t>은둔자</t>
+  </si>
+  <si>
+    <t>어떤 이유에서인지 모르지만, 대부분의 사람들은 {PAWN_nameDef}(이)가 어떤 기분을 느끼는지를 생생히 느낄 수 있는 듯 합니다.</t>
+  </si>
+  <si>
+    <t>선각자</t>
+  </si>
+  <si>
+    <t>열정적인</t>
+  </si>
+  <si>
+    <t>속좁은</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 천제적인 재능을 타고난 제작자이며, 종종 창의적인 영감을 받습니다. 하지만 {PAWN_pronoun}의 마음은 끊임없이 새로운 것을 추구하며, 때문에 정신적인 단절을 훨씬 자주 일으킵니다.</t>
+  </si>
+  <si>
+    <t>휘발성 창의력</t>
   </si>
   <si>
     <t>{PAWN_nameDef}(은)는 다른 사람의 행동에 가혹하게 비판하고 지시합니다. {PAWN_nameDef}의 근처에 있는 정착민들은 더 빠르게 움직이고 작업하지만, 받는 스트레스가 늘어납니다.</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 위험을 감수하고 임무를 완수하기를 좋아합니다. {PAWN_pronoun} 임무가 성공적일 때 기분이 좋아지며, 실패한 임무에는 기분이 나빠집니다.</t>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 사회적인 우열에 매우 관심이 있습니다. {PAWN_pronoun}(은)는 다른 사람들을 괴롭히는 경향이 있으며, {PAWN_pronoun}의 전 연인들이 그 주요 대상입니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{PAWN_nameDef}(은)는 위험을 감수하고 임무를 완수하기를 좋아합니다. {PAWN_pronoun} 임무가 성공적일 때 기분이 좋아지며, 실패한 임무에는 기분이 나빠집니다.</t>
+    <t>{PAWN_nameDef}(은)는 후광처럼 빛나는 매력을 지니고 있습니다. {PAWN_pronoun}의 말은 다른 사람들보다 더욱 큰 영향력을 끼치며, 그들은 {PAWN_pronoun}(을)를 더욱 가깝게 느낄 것입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 매우 비정상적으로 행동합니다. 아마도 지능에 문제가 있을 수 있습니다. {PAWN_pronoun}(은)는 종종 사회적으로 큰 영향을 끼칩니다. 좋거나, 나쁘거나요. {PAWN_nameDef}의 사교적 감각은 너무 나빠서, {PAWN_pronoun}(은)는 누군가 자신을 모욕하는걸 잘 깨닫지 못합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 독방을 선호합니다. 또한 {PAWN_pronoun}(은)는 말이 필요없는 식물들과 함께 있는 것을 더욱 좋아합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 에너지가 넘치는 사람입니다. {PAWN_pronoun}(은)는 행복한 상태가 아니더라도 영감을 자주 얻을 수 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1073,7 +1179,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1121,7 +1227,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1138,7 +1244,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1155,7 +1261,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1172,7 +1278,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1189,7 +1295,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1206,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1223,7 +1329,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1240,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1257,7 +1363,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -1274,7 +1380,7 @@
         <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -1291,7 +1397,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1308,7 +1414,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -1325,7 +1431,7 @@
         <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1342,7 +1448,7 @@
         <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1359,7 +1465,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1376,7 +1482,7 @@
         <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1393,7 +1499,7 @@
         <v>58</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1410,7 +1516,7 @@
         <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1427,7 +1533,7 @@
         <v>64</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1444,7 +1550,7 @@
         <v>67</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1461,7 +1567,7 @@
         <v>70</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1478,7 +1584,7 @@
         <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1495,7 +1601,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -1512,7 +1618,7 @@
         <v>73</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -1529,7 +1635,7 @@
         <v>81</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -1546,7 +1652,7 @@
         <v>73</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -1563,7 +1669,7 @@
         <v>86</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1580,7 +1686,7 @@
         <v>89</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -1597,7 +1703,7 @@
         <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -1614,7 +1720,7 @@
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -1631,7 +1737,7 @@
         <v>98</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -1648,7 +1754,7 @@
         <v>101</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -1665,7 +1771,7 @@
         <v>104</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -1682,7 +1788,7 @@
         <v>101</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -1699,7 +1805,7 @@
         <v>109</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -1716,7 +1822,7 @@
         <v>112</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -1733,7 +1839,7 @@
         <v>115</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -1750,7 +1856,7 @@
         <v>112</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -1767,7 +1873,7 @@
         <v>120</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -1784,7 +1890,7 @@
         <v>112</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -1801,7 +1907,7 @@
         <v>125</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -1818,7 +1924,7 @@
         <v>112</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -1835,7 +1941,7 @@
         <v>130</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -1852,7 +1958,7 @@
         <v>133</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -1869,7 +1975,7 @@
         <v>136</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -1886,7 +1992,7 @@
         <v>140</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -1903,7 +2009,7 @@
         <v>143</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -1920,7 +2026,7 @@
         <v>146</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -1937,7 +2043,7 @@
         <v>149</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -1954,7 +2060,7 @@
         <v>152</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -1971,7 +2077,7 @@
         <v>155</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -1988,7 +2094,7 @@
         <v>158</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2005,7 +2111,7 @@
         <v>161</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
@@ -2016,234 +2122,234 @@
         <v>138</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="F61" s="1" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="F63" s="1" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="F64" s="1" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="F65" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="F66" s="1" t="s">
-        <v>226</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="F68" s="1" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>